<commit_message>
import pyautogui and fix enter
</commit_message>
<xml_diff>
--- a/excel/list.xlsx
+++ b/excel/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KIMPOFD9\Documents\GitHub\fms-auto\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F08A9F-10A1-44B4-9298-0D73BA2A7692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0195FF70-216B-4561-9B22-88B729291A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>shop</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,6 +40,218 @@
   </si>
   <si>
     <t>cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0625</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0702</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>171800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0623</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>52600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0626</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>404800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0703</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>273800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>126</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>338700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0624</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>306</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>634300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>137</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>285500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>481</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>985900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>35500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>274300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0706</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0629</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>166</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>331000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>138500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0630</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0705</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -393,6 +605,244 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>